<commit_message>
Update RGB LED resistor calculations.xlsx
</commit_message>
<xml_diff>
--- a/RGB LED resistor calculations.xlsx
+++ b/RGB LED resistor calculations.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/783aa649d406c4c9/Documents/GitHub/Programming/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_3A53D2B7090F6530070B66432EFC3873AB875007" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F7D56A-E2D0-4054-85FB-DA6A350C7C1C}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="300" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,18 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$F$8</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -57,9 +73,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -190,7 +206,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,9 +221,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -218,6 +231,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -232,6 +257,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -556,36 +589,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.75" style="12" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="20">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="45">
+    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -595,7 +628,7 @@
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -605,15 +638,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>9</v>
       </c>
@@ -623,19 +656,19 @@
       <c r="C5" s="5">
         <v>2.1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="13">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E5" s="5">
         <f>A5-C5</f>
         <v>6.9</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f>E5/D5</f>
         <v>383.33333333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>9</v>
       </c>
@@ -645,19 +678,19 @@
       <c r="C6" s="5">
         <v>3.1</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="13">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" ref="E6:E7" si="0">A6-C6</f>
         <v>5.9</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f t="shared" ref="F6:F7" si="1">E6/D6</f>
         <v>327.77777777777783</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>9</v>
       </c>
@@ -667,23 +700,23 @@
       <c r="C7" s="5">
         <v>3.1</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="13">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>5.9</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>327.77777777777783</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>

</xml_diff>